<commit_message>
Mat Price als Faktor und Feature
</commit_message>
<xml_diff>
--- a/Mat_Price_Test_Test/2600038/features.xlsx
+++ b/Mat_Price_Test_Test/2600038/features.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:V61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,6 +473,81 @@
           <t>Price_Material_var</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>EoD_Bestand_noSiBe_log1p</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>DeficitPos_log1p</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>DemandMean_100_log1p</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>DemandMax_100_log1p</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>DemandMean_66_log1p</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>DemandMax_66_log1p</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>DemandMean_50_log1p</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>DemandMax_50_log1p</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>DemandMean_25_log1p</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>DemandMax_25_log1p</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Lag_EoD_Bestand_noSiBe_mean_7Tage</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Lag_EoD_Bestand_noSiBe_mean_28Tage</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Lag_EoD_Bestand_noSiBe_mean_wbzTage</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Lag_EoD_Bestand_noSiBe_mean_2xwbzTage</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>L_WBZ_BlockMinAbs</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -495,7 +570,54 @@
       <c r="F2" t="n">
         <v>14</v>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H2" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1617.178571428571</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1617.178571428571</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -518,7 +640,54 @@
       <c r="F3" t="n">
         <v>14</v>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H3" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1613.785714285714</v>
+      </c>
+      <c r="T3" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U3" t="n">
+        <v>1613.785714285714</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -541,7 +710,54 @@
       <c r="F4" t="n">
         <v>14</v>
       </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H4" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1610.392857142857</v>
+      </c>
+      <c r="T4" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U4" t="n">
+        <v>1610.392857142857</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -564,7 +780,54 @@
       <c r="F5" t="n">
         <v>14</v>
       </c>
-      <c r="G5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H5" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U5" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -587,7 +850,54 @@
       <c r="F6" t="n">
         <v>14</v>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H6" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T6" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U6" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -610,7 +920,54 @@
       <c r="F7" t="n">
         <v>14</v>
       </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H7" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T7" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U7" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -633,7 +990,54 @@
       <c r="F8" t="n">
         <v>14</v>
       </c>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H8" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T8" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U8" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -656,7 +1060,54 @@
       <c r="F9" t="n">
         <v>14</v>
       </c>
-      <c r="G9" t="inlineStr"/>
+      <c r="G9" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H9" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T9" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U9" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -679,7 +1130,54 @@
       <c r="F10" t="n">
         <v>14</v>
       </c>
-      <c r="G10" t="inlineStr"/>
+      <c r="G10" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H10" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S10" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T10" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U10" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -702,7 +1200,54 @@
       <c r="F11" t="n">
         <v>14</v>
       </c>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H11" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S11" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T11" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U11" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -725,7 +1270,54 @@
       <c r="F12" t="n">
         <v>14</v>
       </c>
-      <c r="G12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H12" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T12" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U12" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -748,7 +1340,54 @@
       <c r="F13" t="n">
         <v>14</v>
       </c>
-      <c r="G13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H13" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S13" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T13" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U13" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -771,7 +1410,54 @@
       <c r="F14" t="n">
         <v>14</v>
       </c>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H14" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S14" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T14" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U14" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -794,7 +1480,54 @@
       <c r="F15" t="n">
         <v>14</v>
       </c>
-      <c r="G15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H15" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T15" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U15" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -817,7 +1550,54 @@
       <c r="F16" t="n">
         <v>14</v>
       </c>
-      <c r="G16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H16" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S16" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T16" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U16" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -840,7 +1620,54 @@
       <c r="F17" t="n">
         <v>14</v>
       </c>
-      <c r="G17" t="inlineStr"/>
+      <c r="G17" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H17" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S17" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T17" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U17" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -863,7 +1690,54 @@
       <c r="F18" t="n">
         <v>14</v>
       </c>
-      <c r="G18" t="inlineStr"/>
+      <c r="G18" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H18" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S18" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T18" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U18" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -886,7 +1760,54 @@
       <c r="F19" t="n">
         <v>14</v>
       </c>
-      <c r="G19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H19" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S19" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T19" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U19" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -909,7 +1830,54 @@
       <c r="F20" t="n">
         <v>14</v>
       </c>
-      <c r="G20" t="inlineStr"/>
+      <c r="G20" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H20" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S20" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T20" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U20" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -932,7 +1900,54 @@
       <c r="F21" t="n">
         <v>14</v>
       </c>
-      <c r="G21" t="inlineStr"/>
+      <c r="G21" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H21" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S21" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T21" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U21" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -955,7 +1970,54 @@
       <c r="F22" t="n">
         <v>14</v>
       </c>
-      <c r="G22" t="inlineStr"/>
+      <c r="G22" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H22" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S22" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T22" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U22" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -978,7 +2040,54 @@
       <c r="F23" t="n">
         <v>14</v>
       </c>
-      <c r="G23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H23" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S23" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T23" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U23" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1001,7 +2110,54 @@
       <c r="F24" t="n">
         <v>14</v>
       </c>
-      <c r="G24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H24" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S24" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T24" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U24" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1024,7 +2180,54 @@
       <c r="F25" t="n">
         <v>14</v>
       </c>
-      <c r="G25" t="inlineStr"/>
+      <c r="G25" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H25" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S25" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T25" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U25" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1047,7 +2250,54 @@
       <c r="F26" t="n">
         <v>14</v>
       </c>
-      <c r="G26" t="inlineStr"/>
+      <c r="G26" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H26" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S26" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T26" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U26" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1070,7 +2320,54 @@
       <c r="F27" t="n">
         <v>14</v>
       </c>
-      <c r="G27" t="inlineStr"/>
+      <c r="G27" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H27" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S27" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T27" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U27" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1093,7 +2390,54 @@
       <c r="F28" t="n">
         <v>14</v>
       </c>
-      <c r="G28" t="inlineStr"/>
+      <c r="G28" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H28" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S28" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T28" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U28" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1116,7 +2460,54 @@
       <c r="F29" t="n">
         <v>14</v>
       </c>
-      <c r="G29" t="inlineStr"/>
+      <c r="G29" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H29" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S29" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T29" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U29" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1139,7 +2530,54 @@
       <c r="F30" t="n">
         <v>14</v>
       </c>
-      <c r="G30" t="inlineStr"/>
+      <c r="G30" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H30" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S30" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T30" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U30" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1162,7 +2600,54 @@
       <c r="F31" t="n">
         <v>14</v>
       </c>
-      <c r="G31" t="inlineStr"/>
+      <c r="G31" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H31" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S31" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T31" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U31" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1185,7 +2670,54 @@
       <c r="F32" t="n">
         <v>14</v>
       </c>
-      <c r="G32" t="inlineStr"/>
+      <c r="G32" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H32" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S32" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T32" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U32" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1208,7 +2740,54 @@
       <c r="F33" t="n">
         <v>14</v>
       </c>
-      <c r="G33" t="inlineStr"/>
+      <c r="G33" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H33" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S33" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T33" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U33" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1231,7 +2810,54 @@
       <c r="F34" t="n">
         <v>14</v>
       </c>
-      <c r="G34" t="inlineStr"/>
+      <c r="G34" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H34" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S34" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T34" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U34" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1254,7 +2880,54 @@
       <c r="F35" t="n">
         <v>14</v>
       </c>
-      <c r="G35" t="inlineStr"/>
+      <c r="G35" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H35" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S35" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T35" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U35" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1277,7 +2950,54 @@
       <c r="F36" t="n">
         <v>14</v>
       </c>
-      <c r="G36" t="inlineStr"/>
+      <c r="G36" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H36" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S36" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T36" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U36" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1300,7 +3020,54 @@
       <c r="F37" t="n">
         <v>14</v>
       </c>
-      <c r="G37" t="inlineStr"/>
+      <c r="G37" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H37" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S37" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T37" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U37" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1323,7 +3090,54 @@
       <c r="F38" t="n">
         <v>14</v>
       </c>
-      <c r="G38" t="inlineStr"/>
+      <c r="G38" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H38" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S38" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T38" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U38" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1346,7 +3160,54 @@
       <c r="F39" t="n">
         <v>14</v>
       </c>
-      <c r="G39" t="inlineStr"/>
+      <c r="G39" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H39" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S39" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T39" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U39" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1369,7 +3230,54 @@
       <c r="F40" t="n">
         <v>14</v>
       </c>
-      <c r="G40" t="inlineStr"/>
+      <c r="G40" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H40" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0</v>
+      </c>
+      <c r="P40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>0</v>
+      </c>
+      <c r="R40" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S40" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T40" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U40" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1392,7 +3300,54 @@
       <c r="F41" t="n">
         <v>14</v>
       </c>
-      <c r="G41" t="inlineStr"/>
+      <c r="G41" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H41" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" t="n">
+        <v>0</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S41" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T41" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U41" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1415,7 +3370,54 @@
       <c r="F42" t="n">
         <v>14</v>
       </c>
-      <c r="G42" t="inlineStr"/>
+      <c r="G42" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H42" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S42" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T42" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U42" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1438,7 +3440,54 @@
       <c r="F43" t="n">
         <v>14</v>
       </c>
-      <c r="G43" t="inlineStr"/>
+      <c r="G43" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H43" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S43" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T43" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U43" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1461,7 +3510,54 @@
       <c r="F44" t="n">
         <v>14</v>
       </c>
-      <c r="G44" t="inlineStr"/>
+      <c r="G44" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H44" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0</v>
+      </c>
+      <c r="P44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>0</v>
+      </c>
+      <c r="R44" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S44" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T44" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U44" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1484,7 +3580,54 @@
       <c r="F45" t="n">
         <v>14</v>
       </c>
-      <c r="G45" t="inlineStr"/>
+      <c r="G45" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H45" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>0</v>
+      </c>
+      <c r="R45" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S45" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T45" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U45" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1507,7 +3650,54 @@
       <c r="F46" t="n">
         <v>14</v>
       </c>
-      <c r="G46" t="inlineStr"/>
+      <c r="G46" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H46" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>0</v>
+      </c>
+      <c r="R46" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S46" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T46" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U46" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1530,7 +3720,54 @@
       <c r="F47" t="n">
         <v>14</v>
       </c>
-      <c r="G47" t="inlineStr"/>
+      <c r="G47" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H47" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>0</v>
+      </c>
+      <c r="R47" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S47" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T47" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U47" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1553,7 +3790,54 @@
       <c r="F48" t="n">
         <v>14</v>
       </c>
-      <c r="G48" t="inlineStr"/>
+      <c r="G48" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H48" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" t="n">
+        <v>0</v>
+      </c>
+      <c r="P48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>0</v>
+      </c>
+      <c r="R48" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S48" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T48" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U48" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1576,7 +3860,54 @@
       <c r="F49" t="n">
         <v>14</v>
       </c>
-      <c r="G49" t="inlineStr"/>
+      <c r="G49" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H49" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0</v>
+      </c>
+      <c r="P49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>0</v>
+      </c>
+      <c r="R49" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S49" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T49" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U49" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1599,7 +3930,54 @@
       <c r="F50" t="n">
         <v>14</v>
       </c>
-      <c r="G50" t="inlineStr"/>
+      <c r="G50" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H50" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0</v>
+      </c>
+      <c r="O50" t="n">
+        <v>0</v>
+      </c>
+      <c r="P50" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>0</v>
+      </c>
+      <c r="R50" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S50" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T50" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U50" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1622,7 +4000,54 @@
       <c r="F51" t="n">
         <v>14</v>
       </c>
-      <c r="G51" t="inlineStr"/>
+      <c r="G51" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H51" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" t="n">
+        <v>0</v>
+      </c>
+      <c r="P51" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>0</v>
+      </c>
+      <c r="R51" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S51" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T51" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U51" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1645,7 +4070,54 @@
       <c r="F52" t="n">
         <v>14</v>
       </c>
-      <c r="G52" t="inlineStr"/>
+      <c r="G52" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H52" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0</v>
+      </c>
+      <c r="P52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>0</v>
+      </c>
+      <c r="R52" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S52" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T52" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U52" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1668,7 +4140,54 @@
       <c r="F53" t="n">
         <v>14</v>
       </c>
-      <c r="G53" t="inlineStr"/>
+      <c r="G53" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H53" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0</v>
+      </c>
+      <c r="P53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>0</v>
+      </c>
+      <c r="R53" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S53" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T53" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U53" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1691,7 +4210,54 @@
       <c r="F54" t="n">
         <v>14</v>
       </c>
-      <c r="G54" t="inlineStr"/>
+      <c r="G54" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H54" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0</v>
+      </c>
+      <c r="O54" t="n">
+        <v>0</v>
+      </c>
+      <c r="P54" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>0</v>
+      </c>
+      <c r="R54" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S54" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T54" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U54" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1714,7 +4280,54 @@
       <c r="F55" t="n">
         <v>14</v>
       </c>
-      <c r="G55" t="inlineStr"/>
+      <c r="G55" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H55" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0</v>
+      </c>
+      <c r="O55" t="n">
+        <v>0</v>
+      </c>
+      <c r="P55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>0</v>
+      </c>
+      <c r="R55" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S55" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T55" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U55" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1737,7 +4350,54 @@
       <c r="F56" t="n">
         <v>14</v>
       </c>
-      <c r="G56" t="inlineStr"/>
+      <c r="G56" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H56" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0</v>
+      </c>
+      <c r="O56" t="n">
+        <v>0</v>
+      </c>
+      <c r="P56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>0</v>
+      </c>
+      <c r="R56" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S56" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T56" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U56" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1760,7 +4420,54 @@
       <c r="F57" t="n">
         <v>14</v>
       </c>
-      <c r="G57" t="inlineStr"/>
+      <c r="G57" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H57" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0</v>
+      </c>
+      <c r="M57" t="n">
+        <v>0</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0</v>
+      </c>
+      <c r="O57" t="n">
+        <v>0</v>
+      </c>
+      <c r="P57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>0</v>
+      </c>
+      <c r="R57" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S57" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T57" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U57" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1783,7 +4490,54 @@
       <c r="F58" t="n">
         <v>14</v>
       </c>
-      <c r="G58" t="inlineStr"/>
+      <c r="G58" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H58" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" t="n">
+        <v>0</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>0</v>
+      </c>
+      <c r="R58" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S58" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T58" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U58" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1806,7 +4560,54 @@
       <c r="F59" t="n">
         <v>14</v>
       </c>
-      <c r="G59" t="inlineStr"/>
+      <c r="G59" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H59" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0</v>
+      </c>
+      <c r="O59" t="n">
+        <v>0</v>
+      </c>
+      <c r="P59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q59" t="n">
+        <v>0</v>
+      </c>
+      <c r="R59" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S59" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T59" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U59" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1829,7 +4630,54 @@
       <c r="F60" t="n">
         <v>14</v>
       </c>
-      <c r="G60" t="inlineStr"/>
+      <c r="G60" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H60" t="n">
+        <v>7.382746449738912</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0</v>
+      </c>
+      <c r="N60" t="n">
+        <v>0</v>
+      </c>
+      <c r="O60" t="n">
+        <v>0</v>
+      </c>
+      <c r="P60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q60" t="n">
+        <v>0</v>
+      </c>
+      <c r="R60" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S60" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T60" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U60" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1852,7 +4700,54 @@
       <c r="F61" t="n">
         <v>14</v>
       </c>
-      <c r="G61" t="inlineStr"/>
+      <c r="G61" t="n">
+        <v>0.51837</v>
+      </c>
+      <c r="H61" t="n">
+        <v>6.879355804460439</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q61" t="n">
+        <v>0</v>
+      </c>
+      <c r="R61" t="n">
+        <v>1607</v>
+      </c>
+      <c r="S61" t="n">
+        <v>1607</v>
+      </c>
+      <c r="T61" t="n">
+        <v>1607</v>
+      </c>
+      <c r="U61" t="n">
+        <v>1607</v>
+      </c>
+      <c r="V61" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>